<commit_message>
sudo code for GBDT
</commit_message>
<xml_diff>
--- a/completed_planning/KanbanBoard.xlsx
+++ b/completed_planning/KanbanBoard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkubi\Class Repo\CompanyLocationAndStocks\completed_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79A43F0-D562-45F6-9960-F80CE00DB86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2175B35D-82AF-4A4B-8473-FD1A7EDD7EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28830" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{D25F1752-74CA-430B-B49F-3DA33619D7C0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Story/Task</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>GBDT - sklearn ML</t>
+  </si>
+  <si>
+    <t>Gra</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,9 @@
         <v>27</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
trying to get query to move up
</commit_message>
<xml_diff>
--- a/completed_planning/KanbanBoard.xlsx
+++ b/completed_planning/KanbanBoard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkubi\Class Repo\CompanyLocationAndStocks\completed_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2175B35D-82AF-4A4B-8473-FD1A7EDD7EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F7D0F7-8491-46C8-88D9-6882FA079B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28830" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{D25F1752-74CA-430B-B49F-3DA33619D7C0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Story/Task</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Cleaning up</t>
-  </si>
-  <si>
-    <t>Peer Reviews</t>
   </si>
   <si>
     <t xml:space="preserve">ML Model Needs to be started
@@ -124,7 +121,16 @@
     <t>GBDT - sklearn ML</t>
   </si>
   <si>
-    <t>Gra</t>
+    <t>have reading from postgreSQL complete</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Peer Review Needed</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -194,12 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -525,285 +530,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CC06E2-68E6-42CA-95A1-EAAB6D30F228}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
most of the logic ready
</commit_message>
<xml_diff>
--- a/completed_planning/KanbanBoard.xlsx
+++ b/completed_planning/KanbanBoard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkubi\Class Repo\CompanyLocationAndStocks\completed_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F7D0F7-8491-46C8-88D9-6882FA079B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A32F5F-8D67-4A49-BC48-44F3721D85C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28830" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{D25F1752-74CA-430B-B49F-3DA33619D7C0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Story/Task</t>
   </si>
@@ -47,100 +47,115 @@
     <t>Cleaning up</t>
   </si>
   <si>
-    <t xml:space="preserve">ML Model Needs to be started
-1) read SQL into dataframe
-2) create the SQL
-3)
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Armondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML Random Forest </t>
+  </si>
+  <si>
+    <t>Nikita</t>
+  </si>
+  <si>
+    <t>Research and Mockup of Dash Board</t>
+  </si>
+  <si>
+    <t>Naming all the places where we can find dashboard</t>
+  </si>
+  <si>
+    <t>Research where/how to get SQL to DF</t>
+  </si>
+  <si>
+    <t>Armondo/Kim</t>
+  </si>
+  <si>
+    <t>Kim/Nikita</t>
+  </si>
+  <si>
+    <t>temp (merging all fields together)</t>
+  </si>
+  <si>
+    <t>change stockprice.csv to table name</t>
+  </si>
+  <si>
+    <t>correcting the tables and the testing files</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>Read Deliveralble 2</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kim </t>
+  </si>
+  <si>
+    <t>Nikita/Sarah/Alexis</t>
+  </si>
+  <si>
+    <t>GBDT - sklearn ML</t>
+  </si>
+  <si>
+    <t>have reading from postgreSQL complete</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Peer Review Needed</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>all of us set up tables
+and temp (merging all fields together)</t>
+  </si>
+  <si>
+    <t>Sat???</t>
+  </si>
+  <si>
+    <t>ZOOM MEETING
+get Alexis up to speed on Sunday - 12 PM (about the tables)</t>
+  </si>
+  <si>
+    <t>Alexis_crooks@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>Assignment</t>
-  </si>
-  <si>
-    <t>Kim</t>
-  </si>
-  <si>
-    <t>Armondo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ML Random Forest </t>
-  </si>
-  <si>
-    <t>Nikita</t>
-  </si>
-  <si>
-    <t>Research and Mockup of Dash Board</t>
-  </si>
-  <si>
-    <t>Naming all the places where we can find dashboard</t>
-  </si>
-  <si>
-    <t>Research where/how to get SQL to DF</t>
-  </si>
-  <si>
-    <t>Armondo/Kim</t>
-  </si>
-  <si>
-    <t>Kim/Nikita</t>
-  </si>
-  <si>
-    <t>temp (merging all fields together)</t>
-  </si>
-  <si>
-    <t>change stockprice.csv to table name</t>
-  </si>
-  <si>
-    <t>correcting the tables and the testing files</t>
-  </si>
-  <si>
-    <t>1) all of us set up tables
-and temp (merging all fields together)</t>
-  </si>
-  <si>
-    <t>TEAM</t>
-  </si>
-  <si>
-    <t>Read Deliveralble 2</t>
-  </si>
-  <si>
-    <t>README</t>
-  </si>
-  <si>
-    <t>Alexis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kim </t>
-  </si>
-  <si>
-    <t>Nikita/Sarah/Alexis</t>
-  </si>
-  <si>
-    <t>get Alexis up to speed on Sunday - 12 PM (about the tables)</t>
-  </si>
-  <si>
-    <t>GBDT - sklearn ML</t>
-  </si>
-  <si>
-    <t>have reading from postgreSQL complete</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Peer Review Needed</t>
-  </si>
-  <si>
-    <t>DONE</t>
+    <t>Presentations are drafted in Google Slides.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -196,11 +211,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,8 +243,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,7 +563,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +578,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -557,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -568,11 +598,11 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -580,11 +610,11 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -592,24 +622,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -617,11 +647,11 @@
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -629,37 +659,37 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -668,73 +698,88 @@
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -756,10 +801,10 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -847,6 +892,10 @@
       <c r="F29" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C14" r:id="rId1" display="mailto:Alexis_crooks@yahoo.com" xr:uid="{D6995775-E024-4828-A75E-380195F14DAC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>